<commit_message>
Adición crédito img 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/SolicitudGrafica_CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/SolicitudGrafica_CN_06_04_CO.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
+    <workbookView xWindow="8480" yWindow="3920" windowWidth="29360" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="140001" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -660,25 +660,16 @@
     <t>Hongos</t>
   </si>
   <si>
-    <t>http://recursostic.educacion.es/secundaria/edad/2esobiologia/2quincena7/actividades/estomas.jpg</t>
-  </si>
-  <si>
     <t>Estomas</t>
   </si>
   <si>
     <t>Cloroplastos</t>
   </si>
   <si>
-    <t>http://nuvesa.com.mx/img/diagrama_xilema.png</t>
-  </si>
-  <si>
     <t>Xilema y floema</t>
   </si>
   <si>
     <t>Animal comiendo</t>
-  </si>
-  <si>
-    <t>http://bibliotecadigital.ilce.edu.mx/sites/telesecundaria/tsa03g01v02/imgs/032-06.gif</t>
   </si>
   <si>
     <t>Respiración en peces</t>
@@ -708,6 +699,16 @@
   </si>
   <si>
     <t>Organizar las imágenes con el texto y el formato de esta imagen de referencia:</t>
+  </si>
+  <si>
+    <t>Credito imagen 199771529 Para uso editorial exclusivamente. Queda prohibido el uso de esta imagen para propósitos promocionales o de publicidad. 
+Crédito Editorial: Vipavlenkoff / Shutterstock.com</t>
+  </si>
+  <si>
+    <t>Muestra http://recursostic.educacion.es/secundaria/edad/2esobiologia/2quincena7/actividades/estomas.jpg</t>
+  </si>
+  <si>
+    <t>Muestras http://bibliotecadigital.ilce.edu.mx/sites/telesecundaria/tsa03g01v02/imgs/032-06.gif</t>
   </si>
 </sst>
 </file>
@@ -717,7 +718,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -891,6 +892,11 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1143,11 +1149,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1156,7 +1162,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1164,17 +1170,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1184,7 +1190,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1192,12 +1198,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1206,18 +1212,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1247,11 +1253,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1261,10 +1267,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1274,7 +1280,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1348,16 +1354,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1365,23 +1371,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1443,7 +1449,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1746,6 +1752,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1928,14 +1937,14 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
             <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -1945,7 +1954,7 @@
               <a:tailEnd/>
             </a14:hiddenLine>
           </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -2044,14 +2053,14 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
             <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -2061,7 +2070,7 @@
               <a:tailEnd/>
             </a14:hiddenLine>
           </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -2125,13 +2134,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>962025</xdr:rowOff>
+          <xdr:rowOff>965200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>2028825</xdr:colOff>
+          <xdr:colOff>2032000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>1419225</xdr:rowOff>
+          <xdr:rowOff>1422400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2166,13 +2175,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>2019300</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>962025</xdr:rowOff>
+          <xdr:rowOff>965200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1657350</xdr:colOff>
+          <xdr:colOff>1663700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>1419225</xdr:rowOff>
+          <xdr:rowOff>1422400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2205,15 +2214,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>962025</xdr:rowOff>
+          <xdr:rowOff>965200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:colOff>1663700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>1419225</xdr:rowOff>
+          <xdr:rowOff>1422400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2246,15 +2255,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>962025</xdr:rowOff>
+          <xdr:rowOff>965200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:colOff>1663700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>1419225</xdr:rowOff>
+          <xdr:rowOff>1422400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2289,13 +2298,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>2066925</xdr:colOff>
+          <xdr:colOff>2070100</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>466725</xdr:rowOff>
+          <xdr:rowOff>469900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2328,15 +2337,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>2085975</xdr:colOff>
+          <xdr:colOff>2082800</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1724025</xdr:colOff>
+          <xdr:colOff>1727200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>466725</xdr:rowOff>
+          <xdr:rowOff>469900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2369,15 +2378,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>466725</xdr:rowOff>
+          <xdr:rowOff>469900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2730,32 +2739,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="47.25" style="17" customWidth="1"/>
-    <col min="12" max="12" width="20.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="34.83203125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="47.1640625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="10.875" style="2"/>
+    <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2767,7 +2776,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
@@ -2784,7 +2793,7 @@
       <c r="I2" s="47"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2801,7 +2810,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="16.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2822,7 +2831,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="16.5" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2842,7 +2851,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2855,7 +2864,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="31" t="s">
         <v>40</v>
@@ -2873,7 +2882,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2893,7 +2902,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="26.25" thickBot="1">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
@@ -2928,19 +2937,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="108.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="77" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C10" s="26" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>149</v>
@@ -2965,10 +2974,10 @@
         <v>170</v>
       </c>
       <c r="K10" s="78" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="146.25" customHeight="1">
       <c r="A11" s="13" t="s">
         <v>148</v>
       </c>
@@ -2980,7 +2989,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>149</v>
@@ -3008,7 +3017,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="27">
       <c r="A12" s="73" t="s">
         <v>150</v>
       </c>
@@ -3048,7 +3057,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="40.5">
       <c r="A13" s="73" t="s">
         <v>151</v>
       </c>
@@ -3088,7 +3097,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="15">
       <c r="A14" s="73" t="s">
         <v>152</v>
       </c>
@@ -3126,11 +3135,11 @@
       </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="65">
       <c r="A15" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="13" t="s">
         <v>181</v>
       </c>
       <c r="C15" s="26" t="str">
@@ -3162,9 +3171,11 @@
       <c r="J15" s="74" t="s">
         <v>182</v>
       </c>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="114" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="201" customHeight="1">
       <c r="A16" s="73" t="s">
         <v>154</v>
       </c>
@@ -3204,7 +3215,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A17" s="73" t="s">
         <v>155</v>
       </c>
@@ -3242,7 +3253,7 @@
       </c>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="247.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="247.5" customHeight="1">
       <c r="A18" s="73" t="s">
         <v>156</v>
       </c>
@@ -3282,7 +3293,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="111" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="111">
       <c r="A19" s="73" t="s">
         <v>157</v>
       </c>
@@ -3320,7 +3331,7 @@
       </c>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A20" s="73" t="s">
         <v>158</v>
       </c>
@@ -3358,7 +3369,7 @@
       </c>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A21" s="73" t="s">
         <v>159</v>
       </c>
@@ -3396,7 +3407,7 @@
       </c>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="12" customFormat="1" ht="54">
       <c r="A22" s="73" t="s">
         <v>160</v>
       </c>
@@ -3433,22 +3444,22 @@
         <v>193</v>
       </c>
       <c r="K22" s="82" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="337.5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="12" customFormat="1" ht="342">
       <c r="A23" s="73" t="s">
         <v>161</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C23" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>149</v>
@@ -3473,15 +3484,15 @@
         <v>194</v>
       </c>
       <c r="K23" s="72" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="12" customFormat="1" ht="78.75" customHeight="1">
       <c r="A24" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="B24" s="77" t="s">
-        <v>195</v>
+      <c r="B24" s="77">
+        <v>71038528</v>
       </c>
       <c r="C24" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3510,11 +3521,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="12" customFormat="1">
       <c r="A25" s="73" t="s">
         <v>163</v>
       </c>
@@ -3548,16 +3561,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K25" s="19"/>
     </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A26" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="77" t="s">
-        <v>198</v>
+      <c r="B26" s="77">
+        <v>157035056</v>
       </c>
       <c r="C26" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3586,11 +3599,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="76" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A27" s="73" t="s">
         <v>165</v>
       </c>
@@ -3624,16 +3637,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J27" s="72" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="40">
       <c r="A28" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="B28" s="77" t="s">
-        <v>201</v>
+      <c r="B28" s="77">
+        <v>121635004</v>
       </c>
       <c r="C28" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3662,11 +3675,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J28" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="K28" s="72"/>
-    </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="12" customFormat="1">
       <c r="A29" s="73"/>
       <c r="B29" s="73"/>
       <c r="C29" s="26"/>
@@ -3691,7 +3706,7 @@
       <c r="J29" s="72"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="12" customFormat="1">
       <c r="A30" s="73"/>
       <c r="B30" s="73"/>
       <c r="C30" s="26"/>
@@ -3716,7 +3731,7 @@
       <c r="J30" s="72"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="12" customFormat="1">
       <c r="A31" s="73"/>
       <c r="B31" s="73"/>
       <c r="C31" s="26"/>
@@ -3741,7 +3756,7 @@
       <c r="J31" s="72"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="12" customFormat="1">
       <c r="A32" s="73"/>
       <c r="B32" s="73"/>
       <c r="C32" s="26"/>
@@ -3766,7 +3781,7 @@
       <c r="J32" s="72"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="12" customFormat="1">
       <c r="A33" s="73"/>
       <c r="B33" s="13"/>
       <c r="C33" s="26" t="str">
@@ -3794,7 +3809,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A34" s="13" t="str">
         <f t="shared" ref="A34:A83" si="3">IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),CONCATENATE(LEFT(A33,3),IF(MID(A33,4,2)+1&lt;10,CONCATENATE("0",MID(A33,4,2)+1),MID(A33,4,2)+1)),"")</f>
         <v/>
@@ -3825,7 +3840,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A35" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3856,7 +3871,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A36" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3887,7 +3902,7 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A37" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3918,7 +3933,7 @@
       <c r="J37" s="21"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A38" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3949,7 +3964,7 @@
       <c r="J38" s="22"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A39" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3980,7 +3995,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A40" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4011,7 +4026,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A41" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4042,7 +4057,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A42" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4073,7 +4088,7 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A43" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4104,7 +4119,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A44" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4135,7 +4150,7 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A45" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4166,7 +4181,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A46" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4197,7 +4212,7 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A47" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4228,7 +4243,7 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A48" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4259,7 +4274,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A49" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4290,7 +4305,7 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A50" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4321,7 +4336,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A51" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4352,7 +4367,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A52" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4383,7 +4398,7 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A53" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4414,7 +4429,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A54" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4445,7 +4460,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A55" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4476,7 +4491,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A56" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4507,7 +4522,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A57" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4538,7 +4553,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A58" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4569,7 +4584,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A59" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4600,7 +4615,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A60" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4631,7 +4646,7 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A61" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4662,7 +4677,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A62" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4693,7 +4708,7 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A63" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4724,7 +4739,7 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A64" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4755,7 +4770,7 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A65" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4786,7 +4801,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A66" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4817,7 +4832,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A67" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4848,7 +4863,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A68" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4879,7 +4894,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A69" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4910,7 +4925,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A70" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4941,7 +4956,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A71" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4972,7 +4987,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A72" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5003,7 +5018,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A73" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5034,7 +5049,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A74" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5065,7 +5080,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A75" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5096,7 +5111,7 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A76" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5127,7 +5142,7 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A77" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5158,7 +5173,7 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A78" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5189,7 +5204,7 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A79" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5220,7 +5235,7 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A80" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5251,7 +5266,7 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A81" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5282,7 +5297,7 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A82" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5313,7 +5328,7 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A83" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5344,7 +5359,7 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A84" s="13" t="str">
         <f t="shared" ref="A84:A108" si="7">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
         <v/>
@@ -5375,7 +5390,7 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A85" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5406,7 +5421,7 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A86" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5437,7 +5452,7 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A87" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5468,7 +5483,7 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A88" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5499,7 +5514,7 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A89" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5530,7 +5545,7 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A90" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5561,7 +5576,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A91" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5592,7 +5607,7 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A92" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5623,7 +5638,7 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A93" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5654,7 +5669,7 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A94" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5685,7 +5700,7 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A95" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5716,7 +5731,7 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A96" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5747,7 +5762,7 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A97" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5778,7 +5793,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A98" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5809,7 +5824,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A99" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5840,7 +5855,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A100" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5871,7 +5886,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A101" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5902,7 +5917,7 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A102" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5933,7 +5948,7 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A103" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5964,7 +5979,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A104" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -5995,7 +6010,7 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A105" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6026,7 +6041,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A106" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6057,7 +6072,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A107" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6088,7 +6103,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="12" customFormat="1" ht="15">
       <c r="A108" s="13" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -6170,8 +6185,8 @@
     <hyperlink ref="B23" r:id="rId1" display="http://image.slidesharecdn.com/deuteromicetes-130213124457-phpapp02/95/deuteromicetes-1-638.jpg?cb=1360781133"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6182,25 +6197,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="29" customWidth="1"/>
-    <col min="2" max="2" width="11" style="29"/>
-    <col min="3" max="3" width="13.875" style="29" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="29" customWidth="1"/>
-    <col min="5" max="7" width="11" style="29"/>
+    <col min="1" max="1" width="72.1640625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="29"/>
+    <col min="3" max="3" width="13.83203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="29" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="29"/>
     <col min="8" max="11" width="11" style="29" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="29"/>
+    <col min="12" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1">
       <c r="A1" s="98" t="s">
         <v>38</v>
       </c>
@@ -6210,7 +6225,7 @@
       <c r="E1" s="99"/>
       <c r="F1" s="100"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="37" t="s">
         <v>42</v>
       </c>
@@ -6222,7 +6237,7 @@
       <c r="E2" s="103"/>
       <c r="F2" s="39"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63">
       <c r="A3" s="40" t="s">
         <v>43</v>
       </c>
@@ -6246,7 +6261,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" s="37" t="s">
         <v>44</v>
       </c>
@@ -6274,7 +6289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1">
       <c r="A5" s="40" t="s">
         <v>45</v>
       </c>
@@ -6301,7 +6316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1">
       <c r="A6" s="37" t="s">
         <v>10</v>
       </c>
@@ -6323,7 +6338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="48" thickBot="1">
       <c r="A7" s="40" t="s">
         <v>11</v>
       </c>
@@ -6350,7 +6365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.25">
       <c r="A8" s="40" t="s">
         <v>53</v>
       </c>
@@ -6369,7 +6384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.25">
       <c r="A9" s="40" t="s">
         <v>12</v>
       </c>
@@ -6388,7 +6403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1">
       <c r="A10" s="41" t="s">
         <v>36</v>
       </c>
@@ -6407,7 +6422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="I11" s="29" t="s">
         <v>32</v>
       </c>
@@ -6418,7 +6433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1">
       <c r="I12" s="29" t="s">
         <v>37</v>
       </c>
@@ -6429,7 +6444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="98" t="s">
         <v>41</v>
       </c>
@@ -6448,7 +6463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1">
       <c r="A14" s="40"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -6465,7 +6480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="37" t="s">
         <v>46</v>
       </c>
@@ -6483,7 +6498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.25" customHeight="1">
       <c r="A16" s="40" t="s">
         <v>47</v>
       </c>
@@ -6507,7 +6522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1">
       <c r="A17" s="37" t="s">
         <v>44</v>
       </c>
@@ -6528,7 +6543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1">
       <c r="A18" s="40" t="s">
         <v>48</v>
       </c>
@@ -6549,7 +6564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="37" t="s">
         <v>10</v>
       </c>
@@ -6568,7 +6583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1">
       <c r="A20" s="41" t="s">
         <v>51</v>
       </c>
@@ -6590,7 +6605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="H21" s="29" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6607,122 +6622,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="K22" s="29">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="K23" s="29">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="K24" s="29">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" s="29">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="K26" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="K27" s="29">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="K28" s="29">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="K29" s="29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="K30" s="29">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="K31" s="29">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="K32" s="29">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11">
       <c r="K33" s="29">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11">
       <c r="K34" s="29">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11">
       <c r="K35" s="29">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11">
       <c r="K36" s="29">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11">
       <c r="K37" s="29">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11">
       <c r="K38" s="29">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11">
       <c r="K39" s="29">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11">
       <c r="K40" s="29">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11">
       <c r="K41" s="29">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11">
       <c r="K42" s="29">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11">
       <c r="K43" s="29">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11">
       <c r="K44" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11">
       <c r="K45" s="29" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6741,169 +6756,182 @@
     <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+            <control shapeId="1030" r:id="rId3" name="Drop Down 6">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>962025</xdr:rowOff>
+                    <xdr:rowOff>965200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>2028825</xdr:colOff>
+                    <xdr:colOff>2032000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>1419225</xdr:rowOff>
+                    <xdr:rowOff>1422400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+            <control shapeId="1031" r:id="rId4" name="Drop Down 7">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>2019300</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>962025</xdr:rowOff>
+                    <xdr:rowOff>965200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>1657350</xdr:colOff>
+                    <xdr:colOff>1663700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>1419225</xdr:rowOff>
+                    <xdr:rowOff>1422400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+            <control shapeId="1032" r:id="rId5" name="Drop Down 8">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>962025</xdr:rowOff>
+                    <xdr:rowOff>965200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:colOff>1663700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>1419225</xdr:rowOff>
+                    <xdr:rowOff>1422400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+            <control shapeId="1035" r:id="rId6" name="Drop Down 11">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>962025</xdr:rowOff>
+                    <xdr:rowOff>965200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:colOff>1663700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>1419225</xdr:rowOff>
+                    <xdr:rowOff>1422400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+            <control shapeId="1026" r:id="rId7" name="Drop Down 2">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>2066925</xdr:colOff>
+                    <xdr:colOff>2070100</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>466725</xdr:rowOff>
+                    <xdr:rowOff>469900</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+            <control shapeId="1028" r:id="rId8" name="Drop Down 4">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>2085975</xdr:colOff>
+                    <xdr:colOff>2082800</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>1724025</xdr:colOff>
+                    <xdr:colOff>1727200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>466725</xdr:rowOff>
+                    <xdr:rowOff>469900</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+            <control shapeId="1029" r:id="rId9" name="Drop Down 5">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>466725</xdr:rowOff>
+                    <xdr:rowOff>469900</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6916,23 +6944,23 @@
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="29" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="29" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="29"/>
-    <col min="5" max="5" width="11.75" style="29" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="29" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="29"/>
+    <col min="5" max="5" width="11.6640625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="29" customWidth="1"/>
     <col min="7" max="7" width="11" style="29" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="29" customWidth="1"/>
-    <col min="9" max="9" width="22.25" style="29" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="29" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="29" customWidth="1"/>
     <col min="11" max="11" width="44.5" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="29"/>
+    <col min="12" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="112" t="s">
         <v>56</v>
       </c>
@@ -6960,7 +6988,7 @@
       <c r="I1" s="113"/>
       <c r="J1" s="113"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="112"/>
       <c r="B2" s="112"/>
       <c r="C2" s="112"/>
@@ -6978,7 +7006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="50" customFormat="1">
       <c r="A3" s="49" t="s">
         <v>69</v>
       </c>
@@ -7002,7 +7030,7 @@
       <c r="I3" s="49"/>
       <c r="J3" s="49"/>
     </row>
-    <row r="4" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="50" customFormat="1">
       <c r="A4" s="51" t="s">
         <v>57</v>
       </c>
@@ -7030,7 +7058,7 @@
       </c>
       <c r="J4" s="51"/>
     </row>
-    <row r="5" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="50" customFormat="1">
       <c r="A5" s="52" t="s">
         <v>77</v>
       </c>
@@ -7058,7 +7086,7 @@
       </c>
       <c r="J5" s="53"/>
     </row>
-    <row r="6" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="50" customFormat="1">
       <c r="A6" s="51" t="s">
         <v>58</v>
       </c>
@@ -7090,7 +7118,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="50" customFormat="1" ht="25.5">
       <c r="A7" s="51" t="s">
         <v>80</v>
       </c>
@@ -7118,7 +7146,7 @@
       </c>
       <c r="J7" s="51"/>
     </row>
-    <row r="8" spans="1:11" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="50" customFormat="1" ht="25.5">
       <c r="A8" s="51" t="s">
         <v>82</v>
       </c>
@@ -7146,7 +7174,7 @@
       </c>
       <c r="J8" s="51"/>
     </row>
-    <row r="9" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="50" customFormat="1">
       <c r="A9" s="51" t="s">
         <v>84</v>
       </c>
@@ -7174,7 +7202,7 @@
       </c>
       <c r="J9" s="51"/>
     </row>
-    <row r="10" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="50" customFormat="1">
       <c r="A10" s="51" t="s">
         <v>86</v>
       </c>
@@ -7200,7 +7228,7 @@
       </c>
       <c r="J10" s="51"/>
     </row>
-    <row r="11" spans="1:11" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="50" customFormat="1" ht="25.5">
       <c r="A11" s="51" t="s">
         <v>89</v>
       </c>
@@ -7228,7 +7256,7 @@
       </c>
       <c r="J11" s="51"/>
     </row>
-    <row r="12" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="50" customFormat="1">
       <c r="A12" s="51" t="s">
         <v>91</v>
       </c>
@@ -7256,7 +7284,7 @@
       </c>
       <c r="J12" s="51"/>
     </row>
-    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="63">
       <c r="A13" s="54" t="s">
         <v>93</v>
       </c>
@@ -7283,7 +7311,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="54" t="s">
         <v>97</v>
       </c>
@@ -7307,7 +7335,7 @@
       </c>
       <c r="J14" s="54"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="31.5">
       <c r="A15" s="54" t="s">
         <v>99</v>
       </c>
@@ -7334,7 +7362,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="94.5">
       <c r="A16" s="56" t="s">
         <v>103</v>
       </c>
@@ -7363,7 +7391,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="25.5">
       <c r="A17" s="51" t="s">
         <v>106</v>
       </c>
@@ -7392,12 +7420,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="60" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="61" t="s">
         <v>113</v>
       </c>
@@ -7410,7 +7438,7 @@
       <c r="D21" s="62"/>
       <c r="E21" s="62"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="64" t="s">
         <v>114</v>
       </c>
@@ -7423,7 +7451,7 @@
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="64" t="s">
         <v>115</v>
       </c>
@@ -7436,7 +7464,7 @@
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="31.5">
       <c r="A24" s="64" t="s">
         <v>116</v>
       </c>
@@ -7449,7 +7477,7 @@
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="64" t="s">
         <v>117</v>
       </c>
@@ -7462,7 +7490,7 @@
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
     </row>
-    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="63">
       <c r="A26" s="64" t="s">
         <v>118</v>
       </c>
@@ -7488,5 +7516,10 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>